<commit_message>
working with import data
</commit_message>
<xml_diff>
--- a/api/data/Block 2 Data.xlsx
+++ b/api/data/Block 2 Data.xlsx
@@ -939,13 +939,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="167" formatCode="@"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="#,##0"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1160,28 +1161,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1193,35 +1198,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1241,15 +1242,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1257,11 +1258,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1277,27 +1278,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1309,32 +1310,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1349,39 +1358,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1389,7 +1398,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1397,55 +1406,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1704,83 +1713,83 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q8" activeCellId="0" sqref="Q8"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="9"/>
-    </row>
-    <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="R1" s="10"/>
+    </row>
+    <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="12" t="n">
@@ -1801,7 +1810,7 @@
       <c r="H2" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="16" t="n">
@@ -1830,11 +1839,11 @@
       </c>
       <c r="R2" s="12"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="22" t="n">
@@ -1855,7 +1864,7 @@
       <c r="H3" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="23" t="n">
@@ -1884,11 +1893,11 @@
       </c>
       <c r="R3" s="12"/>
     </row>
-    <row r="4" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+    <row r="4" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="12" t="n">
@@ -1909,7 +1918,7 @@
       <c r="H4" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="16" t="n">
@@ -1938,9 +1947,9 @@
       </c>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="22" t="n">
@@ -1961,7 +1970,7 @@
       <c r="H5" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="26" t="n">
@@ -1990,11 +1999,11 @@
       </c>
       <c r="R5" s="22"/>
     </row>
-    <row r="6" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="22"/>
@@ -2013,7 +2022,7 @@
       <c r="H6" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J6" s="23" t="n">
@@ -2040,11 +2049,11 @@
       <c r="Q6" s="20"/>
       <c r="R6" s="22"/>
     </row>
-    <row r="7" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="22" t="n">
@@ -2063,7 +2072,7 @@
       <c r="H7" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="32"/>
@@ -2089,11 +2098,11 @@
       </c>
       <c r="R7" s="22"/>
     </row>
-    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="22" t="n">
@@ -2114,7 +2123,7 @@
       <c r="H8" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J8" s="23" t="n">
@@ -2143,11 +2152,11 @@
       </c>
       <c r="R8" s="22"/>
     </row>
-    <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="22"/>
@@ -2166,7 +2175,7 @@
       <c r="H9" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J9" s="23"/>
@@ -2190,11 +2199,11 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
     </row>
-    <row r="10" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="22" t="n">
@@ -2215,7 +2224,7 @@
       <c r="H10" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="32"/>
@@ -2241,11 +2250,11 @@
       </c>
       <c r="R10" s="22"/>
     </row>
-    <row r="11" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="22" t="n">
@@ -2266,7 +2275,7 @@
       <c r="H11" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J11" s="32"/>
@@ -2292,11 +2301,11 @@
       </c>
       <c r="R11" s="22"/>
     </row>
-    <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="22" t="n">
@@ -2317,7 +2326,7 @@
       <c r="H12" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J12" s="23" t="n">
@@ -2346,11 +2355,11 @@
       </c>
       <c r="R12" s="22"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="22"/>
@@ -2366,8 +2375,8 @@
       <c r="G13" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="23"/>
       <c r="K13" s="17" t="n">
         <v>92460</v>
@@ -2376,7 +2385,7 @@
         <v>92460</v>
       </c>
       <c r="M13" s="17"/>
-      <c r="N13" s="39" t="s">
+      <c r="N13" s="40" t="s">
         <v>48</v>
       </c>
       <c r="O13" s="17" t="n">
@@ -2391,15 +2400,15 @@
       </c>
       <c r="R13" s="22"/>
     </row>
-    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="40" t="n">
+      <c r="D14" s="41" t="n">
         <v>41276</v>
       </c>
       <c r="E14" s="24" t="n">
@@ -2408,11 +2417,11 @@
       <c r="F14" s="38" t="n">
         <v>120</v>
       </c>
-      <c r="G14" s="40" t="n">
+      <c r="G14" s="41" t="n">
         <v>41276</v>
       </c>
-      <c r="H14" s="40"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="23"/>
       <c r="K14" s="17" t="n">
         <v>75900</v>
@@ -2421,7 +2430,7 @@
         <v>75900</v>
       </c>
       <c r="M14" s="17"/>
-      <c r="N14" s="39" t="s">
+      <c r="N14" s="40" t="s">
         <v>48</v>
       </c>
       <c r="O14" s="17" t="n">
@@ -2436,11 +2445,11 @@
       </c>
       <c r="R14" s="22"/>
     </row>
-    <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22"/>
@@ -2454,8 +2463,8 @@
       <c r="G15" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="13"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="23"/>
       <c r="K15" s="28" t="n">
         <v>55200</v>
@@ -2464,7 +2473,7 @@
         <v>55200</v>
       </c>
       <c r="M15" s="28"/>
-      <c r="N15" s="39" t="n">
+      <c r="N15" s="40" t="n">
         <v>12</v>
       </c>
       <c r="O15" s="28" t="n">
@@ -2478,30 +2487,30 @@
       </c>
       <c r="R15" s="22"/>
     </row>
-    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21"/>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="22"/>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="41" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="36"/>
       <c r="K16" s="36" t="n">
         <f aca="false">SUM(K12:K15)</f>
         <v>230760</v>
       </c>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
       <c r="O16" s="36" t="n">
         <f aca="false">SUM(O12:O15)</f>
         <v>6651360</v>
@@ -2512,11 +2521,11 @@
       <c r="Q16" s="20"/>
       <c r="R16" s="22"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="22" t="n">
@@ -2537,7 +2546,7 @@
       <c r="H17" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J17" s="23" t="n">
@@ -2547,11 +2556,11 @@
         <f aca="false">F17*J17</f>
         <v>26000</v>
       </c>
-      <c r="L17" s="46" t="n">
+      <c r="L17" s="48" t="n">
         <v>26000</v>
       </c>
       <c r="M17" s="17"/>
-      <c r="N17" s="46" t="n">
+      <c r="N17" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O17" s="28" t="n">
@@ -2564,13 +2573,13 @@
       <c r="Q17" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="47"/>
-    </row>
-    <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R17" s="49"/>
+    </row>
+    <row r="18" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="22" t="n">
@@ -2591,7 +2600,7 @@
       <c r="H18" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="23" t="n">
@@ -2605,7 +2614,7 @@
         <v>25000</v>
       </c>
       <c r="M18" s="17"/>
-      <c r="N18" s="46" t="n">
+      <c r="N18" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O18" s="28" t="n">
@@ -2618,13 +2627,13 @@
       <c r="Q18" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="R18" s="47"/>
-    </row>
-    <row r="19" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R18" s="49"/>
+    </row>
+    <row r="19" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="22" t="n">
@@ -2645,7 +2654,7 @@
       <c r="H19" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="23" t="n">
@@ -2659,7 +2668,7 @@
         <v>5000</v>
       </c>
       <c r="M19" s="17"/>
-      <c r="N19" s="46" t="n">
+      <c r="N19" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O19" s="28" t="n">
@@ -2674,11 +2683,11 @@
       </c>
       <c r="R19" s="22"/>
     </row>
-    <row r="20" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="22" t="n">
@@ -2700,7 +2709,7 @@
       <c r="H20" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J20" s="23" t="n">
@@ -2714,7 +2723,7 @@
         <v>26600</v>
       </c>
       <c r="M20" s="17"/>
-      <c r="N20" s="46" t="n">
+      <c r="N20" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O20" s="28" t="n">
@@ -2729,11 +2738,11 @@
       </c>
       <c r="R20" s="22"/>
     </row>
-    <row r="21" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="48" t="s">
+    <row r="21" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="22" t="n">
@@ -2754,7 +2763,7 @@
       <c r="H21" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J21" s="23" t="n">
@@ -2768,7 +2777,7 @@
         <v>21250</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="N21" s="46" t="n">
+      <c r="N21" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O21" s="28" t="n">
@@ -2783,11 +2792,11 @@
       </c>
       <c r="R21" s="22"/>
     </row>
-    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="49" t="s">
+    <row r="22" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="22" t="n">
@@ -2808,7 +2817,7 @@
       <c r="H22" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J22" s="23" t="n">
@@ -2822,7 +2831,7 @@
         <v>12000</v>
       </c>
       <c r="M22" s="17"/>
-      <c r="N22" s="46" t="n">
+      <c r="N22" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O22" s="28" t="n">
@@ -2837,11 +2846,11 @@
       </c>
       <c r="R22" s="22"/>
     </row>
-    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="22" t="n">
@@ -2862,7 +2871,7 @@
       <c r="H23" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J23" s="23" t="n">
@@ -2876,7 +2885,7 @@
         <v>29500</v>
       </c>
       <c r="M23" s="17"/>
-      <c r="N23" s="46" t="n">
+      <c r="N23" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O23" s="28" t="n">
@@ -2891,11 +2900,11 @@
       </c>
       <c r="R23" s="22"/>
     </row>
-    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="22" t="n">
@@ -2916,7 +2925,7 @@
       <c r="H24" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J24" s="23" t="n">
@@ -2930,7 +2939,7 @@
         <v>29500</v>
       </c>
       <c r="M24" s="17"/>
-      <c r="N24" s="46" t="n">
+      <c r="N24" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O24" s="28" t="n">
@@ -2945,11 +2954,11 @@
       </c>
       <c r="R24" s="22"/>
     </row>
-    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="48" t="s">
+    <row r="25" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="22" t="n">
@@ -2970,7 +2979,7 @@
       <c r="H25" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J25" s="23" t="n">
@@ -2984,7 +2993,7 @@
         <v>45900</v>
       </c>
       <c r="M25" s="17"/>
-      <c r="N25" s="46" t="n">
+      <c r="N25" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O25" s="28" t="n">
@@ -2999,11 +3008,11 @@
       </c>
       <c r="R25" s="22"/>
     </row>
-    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="22" t="n">
@@ -3024,7 +3033,7 @@
       <c r="H26" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J26" s="23" t="n">
@@ -3038,7 +3047,7 @@
         <v>15000</v>
       </c>
       <c r="M26" s="17"/>
-      <c r="N26" s="46" t="n">
+      <c r="N26" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O26" s="28" t="n">
@@ -3053,11 +3062,11 @@
       </c>
       <c r="R26" s="22"/>
     </row>
-    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="22" t="n">
@@ -3078,7 +3087,7 @@
       <c r="H27" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J27" s="23" t="n">
@@ -3092,7 +3101,7 @@
         <v>40000</v>
       </c>
       <c r="M27" s="17"/>
-      <c r="N27" s="46" t="n">
+      <c r="N27" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O27" s="28" t="n">
@@ -3107,11 +3116,11 @@
       </c>
       <c r="R27" s="22"/>
     </row>
-    <row r="28" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="48" t="s">
+    <row r="28" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="22" t="n">
@@ -3132,7 +3141,7 @@
       <c r="H28" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J28" s="23" t="n">
@@ -3146,7 +3155,7 @@
         <v>30000</v>
       </c>
       <c r="M28" s="17"/>
-      <c r="N28" s="46" t="n">
+      <c r="N28" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O28" s="28" t="n">
@@ -3161,11 +3170,11 @@
       </c>
       <c r="R28" s="22"/>
     </row>
-    <row r="29" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C29" s="22" t="n">
@@ -3186,7 +3195,7 @@
       <c r="H29" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="I29" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J29" s="23" t="n">
@@ -3200,7 +3209,7 @@
         <v>30000</v>
       </c>
       <c r="M29" s="17"/>
-      <c r="N29" s="46" t="n">
+      <c r="N29" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O29" s="28" t="n">
@@ -3215,11 +3224,11 @@
       </c>
       <c r="R29" s="22"/>
     </row>
-    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="22" t="n">
@@ -3240,7 +3249,7 @@
       <c r="H30" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J30" s="23" t="n">
@@ -3254,7 +3263,7 @@
         <v>43350</v>
       </c>
       <c r="M30" s="17"/>
-      <c r="N30" s="46" t="n">
+      <c r="N30" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O30" s="28" t="n">
@@ -3269,11 +3278,11 @@
       </c>
       <c r="R30" s="22"/>
     </row>
-    <row r="31" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="50" t="s">
+    <row r="31" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="22" t="n">
@@ -3294,7 +3303,7 @@
       <c r="H31" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="I31" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J31" s="23" t="n">
@@ -3308,7 +3317,7 @@
         <v>52275</v>
       </c>
       <c r="M31" s="17"/>
-      <c r="N31" s="46" t="n">
+      <c r="N31" s="48" t="n">
         <v>4</v>
       </c>
       <c r="O31" s="28" t="n">
@@ -3323,11 +3332,11 @@
       </c>
       <c r="R31" s="22"/>
     </row>
-    <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C32" s="22" t="n">
@@ -3348,7 +3357,7 @@
       <c r="H32" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="I32" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J32" s="23" t="n">
@@ -3362,7 +3371,7 @@
         <v>52700</v>
       </c>
       <c r="M32" s="17"/>
-      <c r="N32" s="46" t="n">
+      <c r="N32" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O32" s="28" t="n">
@@ -3377,11 +3386,11 @@
       </c>
       <c r="R32" s="22"/>
     </row>
-    <row r="33" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="51" t="s">
+    <row r="33" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="22" t="n">
@@ -3402,7 +3411,7 @@
       <c r="H33" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="I33" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J33" s="23" t="n">
@@ -3416,7 +3425,7 @@
         <v>61200</v>
       </c>
       <c r="M33" s="17"/>
-      <c r="N33" s="46" t="n">
+      <c r="N33" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O33" s="28" t="n">
@@ -3431,11 +3440,11 @@
       </c>
       <c r="R33" s="22"/>
     </row>
-    <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="52" t="s">
+    <row r="34" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="22" t="n">
@@ -3456,7 +3465,7 @@
       <c r="H34" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J34" s="23" t="n">
@@ -3470,7 +3479,7 @@
         <v>6000</v>
       </c>
       <c r="M34" s="17"/>
-      <c r="N34" s="46" t="n">
+      <c r="N34" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O34" s="28" t="n">
@@ -3485,11 +3494,11 @@
       </c>
       <c r="R34" s="22"/>
     </row>
-    <row r="35" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="22" t="n">
@@ -3510,7 +3519,7 @@
       <c r="H35" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="I35" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J35" s="23" t="n">
@@ -3524,7 +3533,7 @@
         <v>7000</v>
       </c>
       <c r="M35" s="17"/>
-      <c r="N35" s="46" t="n">
+      <c r="N35" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O35" s="28" t="n">
@@ -3539,9 +3548,9 @@
       </c>
       <c r="R35" s="22"/>
     </row>
-    <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="30"/>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="22"/>
@@ -3560,7 +3569,7 @@
       <c r="H36" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J36" s="23" t="n">
@@ -3574,7 +3583,7 @@
         <v>10200</v>
       </c>
       <c r="M36" s="17"/>
-      <c r="N36" s="46" t="n">
+      <c r="N36" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O36" s="28" t="n">
@@ -3587,11 +3596,11 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
     </row>
-    <row r="37" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="22"/>
@@ -3610,7 +3619,7 @@
       <c r="H37" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="I37" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J37" s="23"/>
@@ -3621,7 +3630,7 @@
         <v>25000</v>
       </c>
       <c r="M37" s="17"/>
-      <c r="N37" s="46" t="n">
+      <c r="N37" s="48" t="n">
         <v>5</v>
       </c>
       <c r="O37" s="28" t="n">
@@ -3632,13 +3641,13 @@
         <v>3</v>
       </c>
       <c r="Q37" s="22"/>
-      <c r="R37" s="47"/>
-    </row>
-    <row r="38" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="48" t="s">
+      <c r="R37" s="49"/>
+    </row>
+    <row r="38" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="22" t="n">
@@ -3659,7 +3668,7 @@
       <c r="H38" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="I38" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J38" s="23" t="n">
@@ -3673,7 +3682,7 @@
         <v>4800</v>
       </c>
       <c r="M38" s="17"/>
-      <c r="N38" s="46" t="n">
+      <c r="N38" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O38" s="28" t="n">
@@ -3688,11 +3697,11 @@
       </c>
       <c r="R38" s="22"/>
     </row>
-    <row r="39" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C39" s="22" t="n">
@@ -3713,7 +3722,7 @@
       <c r="H39" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="I39" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J39" s="23" t="n">
@@ -3727,7 +3736,7 @@
         <v>16000</v>
       </c>
       <c r="M39" s="17"/>
-      <c r="N39" s="46" t="n">
+      <c r="N39" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O39" s="28" t="n">
@@ -3742,11 +3751,11 @@
       </c>
       <c r="R39" s="22"/>
     </row>
-    <row r="40" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="22" t="n">
@@ -3767,7 +3776,7 @@
       <c r="H40" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="I40" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J40" s="23" t="n">
@@ -3781,7 +3790,7 @@
         <v>16000</v>
       </c>
       <c r="M40" s="17"/>
-      <c r="N40" s="46" t="n">
+      <c r="N40" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O40" s="28" t="n">
@@ -3796,11 +3805,11 @@
       </c>
       <c r="R40" s="22"/>
     </row>
-    <row r="41" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="52" t="s">
+    <row r="41" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="22" t="n">
@@ -3821,7 +3830,7 @@
       <c r="H41" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J41" s="23" t="n">
@@ -3835,7 +3844,7 @@
         <v>24000</v>
       </c>
       <c r="M41" s="17"/>
-      <c r="N41" s="46" t="n">
+      <c r="N41" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O41" s="28" t="n">
@@ -3850,11 +3859,11 @@
       </c>
       <c r="R41" s="22"/>
     </row>
-    <row r="42" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="22" t="n">
@@ -3875,7 +3884,7 @@
       <c r="H42" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J42" s="23" t="n">
@@ -3889,7 +3898,7 @@
         <v>24000</v>
       </c>
       <c r="M42" s="17"/>
-      <c r="N42" s="46" t="n">
+      <c r="N42" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O42" s="28" t="n">
@@ -3904,11 +3913,11 @@
       </c>
       <c r="R42" s="22"/>
     </row>
-    <row r="43" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="22" t="n">
@@ -3929,7 +3938,7 @@
       <c r="H43" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I43" s="13" t="s">
+      <c r="I43" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J43" s="23" t="n">
@@ -3943,7 +3952,7 @@
         <v>35700</v>
       </c>
       <c r="M43" s="17"/>
-      <c r="N43" s="46" t="n">
+      <c r="N43" s="48" t="n">
         <v>2</v>
       </c>
       <c r="O43" s="28" t="n">
@@ -3956,13 +3965,13 @@
       <c r="Q43" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="R43" s="47"/>
-    </row>
-    <row r="44" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
+      <c r="R43" s="49"/>
+    </row>
+    <row r="44" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C44" s="12" t="n">
@@ -3983,7 +3992,7 @@
       <c r="H44" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I44" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J44" s="23" t="n">
@@ -3997,7 +4006,7 @@
         <v>43260</v>
       </c>
       <c r="M44" s="17"/>
-      <c r="N44" s="46" t="n">
+      <c r="N44" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O44" s="28" t="n">
@@ -4012,11 +4021,11 @@
       </c>
       <c r="R44" s="12"/>
     </row>
-    <row r="45" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="22" t="n">
@@ -4037,7 +4046,7 @@
       <c r="H45" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I45" s="13" t="s">
+      <c r="I45" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J45" s="23" t="n">
@@ -4051,7 +4060,7 @@
         <v>9600</v>
       </c>
       <c r="M45" s="17"/>
-      <c r="N45" s="46" t="n">
+      <c r="N45" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O45" s="28" t="n">
@@ -4064,13 +4073,13 @@
       <c r="Q45" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R45" s="47"/>
-    </row>
-    <row r="46" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="50" t="s">
+      <c r="R45" s="49"/>
+    </row>
+    <row r="46" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C46" s="22" t="n">
@@ -4091,7 +4100,7 @@
       <c r="H46" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="I46" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J46" s="23" t="n">
@@ -4105,7 +4114,7 @@
         <v>59500</v>
       </c>
       <c r="M46" s="17"/>
-      <c r="N46" s="46" t="n">
+      <c r="N46" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O46" s="28" t="n">
@@ -4120,11 +4129,11 @@
       </c>
       <c r="R46" s="22"/>
     </row>
-    <row r="47" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="50" t="s">
+    <row r="47" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="22" t="n">
@@ -4145,7 +4154,7 @@
       <c r="H47" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="I47" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J47" s="23" t="n">
@@ -4159,7 +4168,7 @@
         <v>30400</v>
       </c>
       <c r="M47" s="17"/>
-      <c r="N47" s="46" t="n">
+      <c r="N47" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O47" s="28" t="n">
@@ -4174,11 +4183,11 @@
       </c>
       <c r="R47" s="22"/>
     </row>
-    <row r="48" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="50" t="s">
+    <row r="48" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="22" t="n">
@@ -4199,7 +4208,7 @@
       <c r="H48" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I48" s="13" t="s">
+      <c r="I48" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J48" s="23" t="n">
@@ -4213,7 +4222,7 @@
         <v>19200</v>
       </c>
       <c r="M48" s="17"/>
-      <c r="N48" s="46" t="n">
+      <c r="N48" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O48" s="28" t="n">
@@ -4228,11 +4237,11 @@
       </c>
       <c r="R48" s="22"/>
     </row>
-    <row r="49" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="50" t="s">
+    <row r="49" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C49" s="22" t="n">
@@ -4253,7 +4262,7 @@
       <c r="H49" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I49" s="13" t="s">
+      <c r="I49" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J49" s="23" t="n">
@@ -4267,7 +4276,7 @@
         <v>44100</v>
       </c>
       <c r="M49" s="17"/>
-      <c r="N49" s="46" t="n">
+      <c r="N49" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O49" s="28" t="n">
@@ -4282,9 +4291,9 @@
       </c>
       <c r="R49" s="22"/>
     </row>
-    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="21"/>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C50" s="22"/>
@@ -4303,7 +4312,7 @@
       <c r="H50" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I50" s="13" t="s">
+      <c r="I50" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J50" s="23" t="n">
@@ -4317,7 +4326,7 @@
         <v>2800</v>
       </c>
       <c r="M50" s="17"/>
-      <c r="N50" s="46" t="n">
+      <c r="N50" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O50" s="28" t="n">
@@ -4330,11 +4339,11 @@
       <c r="Q50" s="20"/>
       <c r="R50" s="22"/>
     </row>
-    <row r="51" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="50" t="s">
+    <row r="51" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="22" t="n">
@@ -4355,7 +4364,7 @@
       <c r="H51" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I51" s="13" t="s">
+      <c r="I51" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J51" s="23" t="n">
@@ -4369,7 +4378,7 @@
         <v>23600</v>
       </c>
       <c r="M51" s="17"/>
-      <c r="N51" s="46" t="n">
+      <c r="N51" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O51" s="28" t="n">
@@ -4384,11 +4393,11 @@
       </c>
       <c r="R51" s="22"/>
     </row>
-    <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C52" s="22" t="n">
@@ -4409,7 +4418,7 @@
       <c r="H52" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I52" s="13" t="s">
+      <c r="I52" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J52" s="23" t="n">
@@ -4423,7 +4432,7 @@
         <v>23600</v>
       </c>
       <c r="M52" s="17"/>
-      <c r="N52" s="46" t="n">
+      <c r="N52" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O52" s="28" t="n">
@@ -4438,11 +4447,11 @@
       </c>
       <c r="R52" s="22"/>
     </row>
-    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="22" t="n">
@@ -4463,7 +4472,7 @@
       <c r="H53" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="I53" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J53" s="23" t="n">
@@ -4477,7 +4486,7 @@
         <v>18800</v>
       </c>
       <c r="M53" s="17"/>
-      <c r="N53" s="46" t="n">
+      <c r="N53" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O53" s="28" t="n">
@@ -4492,11 +4501,11 @@
       </c>
       <c r="R53" s="22"/>
     </row>
-    <row r="54" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C54" s="22" t="n">
@@ -4517,7 +4526,7 @@
       <c r="H54" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I54" s="13" t="s">
+      <c r="I54" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J54" s="23" t="n">
@@ -4531,7 +4540,7 @@
         <v>18800</v>
       </c>
       <c r="M54" s="17"/>
-      <c r="N54" s="46" t="n">
+      <c r="N54" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O54" s="28" t="n">
@@ -4544,13 +4553,13 @@
       <c r="Q54" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R54" s="47"/>
-    </row>
-    <row r="55" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="s">
+      <c r="R54" s="49"/>
+    </row>
+    <row r="55" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="22" t="n">
@@ -4571,7 +4580,7 @@
       <c r="H55" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I55" s="13" t="s">
+      <c r="I55" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="23" t="n">
@@ -4585,7 +4594,7 @@
         <v>12000</v>
       </c>
       <c r="M55" s="17"/>
-      <c r="N55" s="46" t="n">
+      <c r="N55" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O55" s="28" t="n">
@@ -4600,11 +4609,11 @@
       </c>
       <c r="R55" s="22"/>
     </row>
-    <row r="56" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="50" t="s">
+    <row r="56" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="22" t="n">
@@ -4625,7 +4634,7 @@
       <c r="H56" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I56" s="13" t="s">
+      <c r="I56" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J56" s="23" t="n">
@@ -4639,7 +4648,7 @@
         <v>5600</v>
       </c>
       <c r="M56" s="17"/>
-      <c r="N56" s="46" t="n">
+      <c r="N56" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O56" s="28" t="n">
@@ -4654,11 +4663,11 @@
       </c>
       <c r="R56" s="22"/>
     </row>
-    <row r="57" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C57" s="22"/>
@@ -4677,7 +4686,7 @@
       <c r="H57" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="I57" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J57" s="23" t="n">
@@ -4691,7 +4700,7 @@
         <v>12000</v>
       </c>
       <c r="M57" s="17"/>
-      <c r="N57" s="46" t="n">
+      <c r="N57" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O57" s="28" t="n">
@@ -4706,11 +4715,11 @@
       </c>
       <c r="R57" s="22"/>
     </row>
-    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="53" t="s">
+    <row r="58" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="22" t="n">
@@ -4731,7 +4740,7 @@
       <c r="H58" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I58" s="13" t="s">
+      <c r="I58" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J58" s="23" t="n">
@@ -4745,7 +4754,7 @@
         <v>42000</v>
       </c>
       <c r="M58" s="17"/>
-      <c r="N58" s="46" t="n">
+      <c r="N58" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O58" s="28" t="n">
@@ -4760,11 +4769,11 @@
       </c>
       <c r="R58" s="22"/>
     </row>
-    <row r="59" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="54" t="s">
+    <row r="59" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="12" t="n">
@@ -4785,7 +4794,7 @@
       <c r="H59" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I59" s="13" t="s">
+      <c r="I59" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J59" s="23" t="n">
@@ -4799,7 +4808,7 @@
         <v>26600</v>
       </c>
       <c r="M59" s="17"/>
-      <c r="N59" s="46" t="n">
+      <c r="N59" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O59" s="28" t="n">
@@ -4814,11 +4823,11 @@
       </c>
       <c r="R59" s="12"/>
     </row>
-    <row r="60" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C60" s="22" t="n">
@@ -4839,7 +4848,7 @@
       <c r="H60" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I60" s="13" t="s">
+      <c r="I60" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J60" s="23" t="n">
@@ -4853,7 +4862,7 @@
         <v>34200</v>
       </c>
       <c r="M60" s="17"/>
-      <c r="N60" s="46" t="n">
+      <c r="N60" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O60" s="28" t="n">
@@ -4868,11 +4877,11 @@
       </c>
       <c r="R60" s="22"/>
     </row>
-    <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C61" s="22" t="n">
@@ -4893,7 +4902,7 @@
       <c r="H61" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I61" s="13" t="s">
+      <c r="I61" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J61" s="23" t="n">
@@ -4907,7 +4916,7 @@
         <v>18200</v>
       </c>
       <c r="M61" s="17"/>
-      <c r="N61" s="46" t="n">
+      <c r="N61" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O61" s="28" t="n">
@@ -4922,11 +4931,11 @@
       </c>
       <c r="R61" s="22"/>
     </row>
-    <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="22" t="n">
@@ -4947,7 +4956,7 @@
       <c r="H62" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I62" s="13" t="s">
+      <c r="I62" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J62" s="23" t="n">
@@ -4961,7 +4970,7 @@
         <v>20300</v>
       </c>
       <c r="M62" s="17"/>
-      <c r="N62" s="46" t="n">
+      <c r="N62" s="48" t="n">
         <v>6</v>
       </c>
       <c r="O62" s="28" t="n">
@@ -4976,11 +4985,11 @@
       </c>
       <c r="R62" s="22"/>
     </row>
-    <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C63" s="22" t="n">
@@ -5001,7 +5010,7 @@
       <c r="H63" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I63" s="13" t="s">
+      <c r="I63" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J63" s="23" t="n">
@@ -5015,7 +5024,7 @@
         <v>30000</v>
       </c>
       <c r="M63" s="17"/>
-      <c r="N63" s="46" t="n">
+      <c r="N63" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O63" s="28" t="n">
@@ -5030,11 +5039,11 @@
       </c>
       <c r="R63" s="22"/>
     </row>
-    <row r="64" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="22" t="n">
@@ -5055,7 +5064,7 @@
       <c r="H64" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I64" s="13" t="s">
+      <c r="I64" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J64" s="23" t="n">
@@ -5069,7 +5078,7 @@
         <v>28840</v>
       </c>
       <c r="M64" s="17"/>
-      <c r="N64" s="46" t="n">
+      <c r="N64" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O64" s="28" t="n">
@@ -5084,11 +5093,11 @@
       </c>
       <c r="R64" s="22"/>
     </row>
-    <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="22" t="n">
@@ -5109,7 +5118,7 @@
       <c r="H65" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I65" s="13" t="s">
+      <c r="I65" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J65" s="23" t="n">
@@ -5123,7 +5132,7 @@
         <v>33600</v>
       </c>
       <c r="M65" s="17"/>
-      <c r="N65" s="46" t="n">
+      <c r="N65" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O65" s="28" t="n">
@@ -5138,11 +5147,11 @@
       </c>
       <c r="R65" s="22"/>
     </row>
-    <row r="66" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="22" t="n">
@@ -5163,7 +5172,7 @@
       <c r="H66" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I66" s="13" t="s">
+      <c r="I66" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J66" s="23" t="n">
@@ -5177,7 +5186,7 @@
         <v>33600</v>
       </c>
       <c r="M66" s="17"/>
-      <c r="N66" s="46" t="n">
+      <c r="N66" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O66" s="28" t="n">
@@ -5192,11 +5201,11 @@
       </c>
       <c r="R66" s="22"/>
     </row>
-    <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C67" s="22" t="n">
@@ -5217,7 +5226,7 @@
       <c r="H67" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I67" s="13" t="s">
+      <c r="I67" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J67" s="23" t="n">
@@ -5231,7 +5240,7 @@
         <v>21000</v>
       </c>
       <c r="M67" s="17"/>
-      <c r="N67" s="46" t="n">
+      <c r="N67" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O67" s="28" t="n">
@@ -5246,11 +5255,11 @@
       </c>
       <c r="R67" s="22"/>
     </row>
-    <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="22" t="n">
@@ -5271,7 +5280,7 @@
       <c r="H68" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I68" s="13" t="s">
+      <c r="I68" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J68" s="23" t="n">
@@ -5285,7 +5294,7 @@
         <v>21000</v>
       </c>
       <c r="M68" s="17"/>
-      <c r="N68" s="46" t="n">
+      <c r="N68" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O68" s="28" t="n">
@@ -5300,11 +5309,11 @@
       </c>
       <c r="R68" s="22"/>
     </row>
-    <row r="69" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="22" t="n">
@@ -5325,7 +5334,7 @@
       <c r="H69" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I69" s="13" t="s">
+      <c r="I69" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J69" s="23" t="n">
@@ -5339,7 +5348,7 @@
         <v>10500</v>
       </c>
       <c r="M69" s="17"/>
-      <c r="N69" s="46" t="n">
+      <c r="N69" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O69" s="28" t="n">
@@ -5354,11 +5363,11 @@
       </c>
       <c r="R69" s="22"/>
     </row>
-    <row r="70" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10" t="s">
+    <row r="70" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C70" s="12" t="n">
@@ -5379,7 +5388,7 @@
       <c r="H70" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I70" s="13" t="s">
+      <c r="I70" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J70" s="23" t="n">
@@ -5389,11 +5398,11 @@
         <f aca="false">F70*J70</f>
         <v>17500</v>
       </c>
-      <c r="L70" s="46" t="n">
+      <c r="L70" s="48" t="n">
         <v>17500</v>
       </c>
       <c r="M70" s="17"/>
-      <c r="N70" s="46" t="n">
+      <c r="N70" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O70" s="28" t="n">
@@ -5408,11 +5417,11 @@
       </c>
       <c r="R70" s="12"/>
     </row>
-    <row r="71" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C71" s="22" t="n">
@@ -5433,7 +5442,7 @@
       <c r="H71" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I71" s="13" t="s">
+      <c r="I71" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J71" s="23" t="n">
@@ -5447,7 +5456,7 @@
         <v>10500</v>
       </c>
       <c r="M71" s="17"/>
-      <c r="N71" s="46" t="n">
+      <c r="N71" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O71" s="28" t="n">
@@ -5462,11 +5471,11 @@
       </c>
       <c r="R71" s="22"/>
     </row>
-    <row r="72" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C72" s="22" t="n">
@@ -5487,7 +5496,7 @@
       <c r="H72" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I72" s="13" t="s">
+      <c r="I72" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J72" s="23" t="n">
@@ -5501,7 +5510,7 @@
         <v>4200</v>
       </c>
       <c r="M72" s="17"/>
-      <c r="N72" s="46" t="n">
+      <c r="N72" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O72" s="28" t="n">
@@ -5516,11 +5525,11 @@
       </c>
       <c r="R72" s="22"/>
     </row>
-    <row r="73" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C73" s="22" t="n">
@@ -5541,7 +5550,7 @@
       <c r="H73" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I73" s="13" t="s">
+      <c r="I73" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J73" s="23" t="n">
@@ -5555,7 +5564,7 @@
         <v>21000</v>
       </c>
       <c r="M73" s="17"/>
-      <c r="N73" s="46" t="n">
+      <c r="N73" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O73" s="28" t="n">
@@ -5570,11 +5579,11 @@
       </c>
       <c r="R73" s="22"/>
     </row>
-    <row r="74" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C74" s="22" t="n">
@@ -5595,7 +5604,7 @@
       <c r="H74" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I74" s="13" t="s">
+      <c r="I74" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J74" s="23" t="n">
@@ -5609,7 +5618,7 @@
         <v>9600</v>
       </c>
       <c r="M74" s="17"/>
-      <c r="N74" s="46" t="n">
+      <c r="N74" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O74" s="28" t="n">
@@ -5624,11 +5633,11 @@
       </c>
       <c r="R74" s="22"/>
     </row>
-    <row r="75" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C75" s="22" t="n">
@@ -5649,7 +5658,7 @@
       <c r="H75" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I75" s="13" t="s">
+      <c r="I75" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J75" s="23" t="n">
@@ -5663,7 +5672,7 @@
         <v>7200</v>
       </c>
       <c r="M75" s="17"/>
-      <c r="N75" s="46" t="n">
+      <c r="N75" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O75" s="28" t="n">
@@ -5678,11 +5687,11 @@
       </c>
       <c r="R75" s="22"/>
     </row>
-    <row r="76" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C76" s="22" t="n">
@@ -5703,7 +5712,7 @@
       <c r="H76" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I76" s="13" t="s">
+      <c r="I76" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J76" s="23" t="n">
@@ -5717,7 +5726,7 @@
         <v>12852</v>
       </c>
       <c r="M76" s="17"/>
-      <c r="N76" s="46" t="n">
+      <c r="N76" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O76" s="28" t="n">
@@ -5732,11 +5741,11 @@
       </c>
       <c r="R76" s="22"/>
     </row>
-    <row r="77" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C77" s="22" t="n">
@@ -5757,7 +5766,7 @@
       <c r="H77" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I77" s="13" t="s">
+      <c r="I77" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J77" s="23" t="n">
@@ -5771,7 +5780,7 @@
         <v>12621</v>
       </c>
       <c r="M77" s="17"/>
-      <c r="N77" s="46" t="n">
+      <c r="N77" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O77" s="28" t="n">
@@ -5786,11 +5795,11 @@
       </c>
       <c r="R77" s="22"/>
     </row>
-    <row r="78" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C78" s="22" t="n">
@@ -5811,7 +5820,7 @@
       <c r="H78" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I78" s="13" t="s">
+      <c r="I78" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J78" s="23" t="n">
@@ -5825,7 +5834,7 @@
         <v>23779</v>
       </c>
       <c r="M78" s="17"/>
-      <c r="N78" s="46" t="n">
+      <c r="N78" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O78" s="28" t="n">
@@ -5840,11 +5849,11 @@
       </c>
       <c r="R78" s="22"/>
     </row>
-    <row r="79" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="s">
+    <row r="79" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C79" s="12" t="n">
@@ -5865,7 +5874,7 @@
       <c r="H79" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I79" s="13" t="s">
+      <c r="I79" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J79" s="23" t="n">
@@ -5879,7 +5888,7 @@
         <v>16800</v>
       </c>
       <c r="M79" s="17"/>
-      <c r="N79" s="46" t="n">
+      <c r="N79" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O79" s="28" t="n">
@@ -5894,11 +5903,11 @@
       </c>
       <c r="R79" s="12"/>
     </row>
-    <row r="80" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C80" s="22" t="n">
@@ -5919,7 +5928,7 @@
       <c r="H80" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I80" s="13" t="s">
+      <c r="I80" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J80" s="23" t="n">
@@ -5933,7 +5942,7 @@
         <v>26705</v>
       </c>
       <c r="M80" s="17"/>
-      <c r="N80" s="46" t="n">
+      <c r="N80" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O80" s="28" t="n">
@@ -5948,11 +5957,11 @@
       </c>
       <c r="R80" s="22"/>
     </row>
-    <row r="81" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C81" s="22" t="n">
@@ -5973,7 +5982,7 @@
       <c r="H81" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I81" s="13" t="s">
+      <c r="I81" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J81" s="23" t="n">
@@ -5987,7 +5996,7 @@
         <v>19138</v>
       </c>
       <c r="M81" s="17"/>
-      <c r="N81" s="46" t="n">
+      <c r="N81" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O81" s="28" t="n">
@@ -6002,11 +6011,11 @@
       </c>
       <c r="R81" s="22"/>
     </row>
-    <row r="82" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C82" s="22" t="n">
@@ -6027,7 +6036,7 @@
       <c r="H82" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I82" s="13" t="s">
+      <c r="I82" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J82" s="23" t="n">
@@ -6041,7 +6050,7 @@
         <v>18557</v>
       </c>
       <c r="M82" s="17"/>
-      <c r="N82" s="46" t="n">
+      <c r="N82" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O82" s="28" t="n">
@@ -6054,13 +6063,13 @@
       <c r="Q82" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R82" s="47"/>
-    </row>
-    <row r="83" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R82" s="49"/>
+    </row>
+    <row r="83" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C83" s="22" t="n">
@@ -6081,7 +6090,7 @@
       <c r="H83" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I83" s="13" t="s">
+      <c r="I83" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J83" s="23" t="n">
@@ -6095,7 +6104,7 @@
         <v>19292</v>
       </c>
       <c r="M83" s="17"/>
-      <c r="N83" s="46" t="n">
+      <c r="N83" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O83" s="28" t="n">
@@ -6110,11 +6119,11 @@
       </c>
       <c r="R83" s="22"/>
     </row>
-    <row r="84" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C84" s="22" t="n">
@@ -6135,7 +6144,7 @@
       <c r="H84" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I84" s="13" t="s">
+      <c r="I84" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J84" s="23" t="n">
@@ -6149,7 +6158,7 @@
         <v>18235</v>
       </c>
       <c r="M84" s="17"/>
-      <c r="N84" s="46" t="n">
+      <c r="N84" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O84" s="28" t="n">
@@ -6164,11 +6173,11 @@
       </c>
       <c r="R84" s="22"/>
     </row>
-    <row r="85" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10" t="s">
+    <row r="85" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="12" t="n">
@@ -6189,7 +6198,7 @@
       <c r="H85" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I85" s="13" t="s">
+      <c r="I85" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J85" s="23" t="n">
@@ -6203,7 +6212,7 @@
         <v>18074</v>
       </c>
       <c r="M85" s="17"/>
-      <c r="N85" s="46" t="n">
+      <c r="N85" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O85" s="28" t="n">
@@ -6218,11 +6227,11 @@
       </c>
       <c r="R85" s="12"/>
     </row>
-    <row r="86" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C86" s="22" t="n">
@@ -6243,7 +6252,7 @@
       <c r="H86" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I86" s="13" t="s">
+      <c r="I86" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J86" s="23" t="n">
@@ -6257,7 +6266,7 @@
         <v>20342</v>
       </c>
       <c r="M86" s="17"/>
-      <c r="N86" s="46" t="n">
+      <c r="N86" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O86" s="28" t="n">
@@ -6272,11 +6281,11 @@
       </c>
       <c r="R86" s="22"/>
     </row>
-    <row r="87" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C87" s="22" t="n">
@@ -6297,7 +6306,7 @@
       <c r="H87" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I87" s="13" t="s">
+      <c r="I87" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J87" s="23" t="n">
@@ -6311,7 +6320,7 @@
         <v>43827</v>
       </c>
       <c r="M87" s="17"/>
-      <c r="N87" s="46" t="n">
+      <c r="N87" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O87" s="28" t="n">
@@ -6326,11 +6335,11 @@
       </c>
       <c r="R87" s="22"/>
     </row>
-    <row r="88" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C88" s="22" t="n">
@@ -6351,7 +6360,7 @@
       <c r="H88" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I88" s="13" t="s">
+      <c r="I88" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J88" s="23" t="n">
@@ -6365,7 +6374,7 @@
         <v>16870</v>
       </c>
       <c r="M88" s="17"/>
-      <c r="N88" s="46" t="n">
+      <c r="N88" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O88" s="28" t="n">
@@ -6380,11 +6389,11 @@
       </c>
       <c r="R88" s="22"/>
     </row>
-    <row r="89" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C89" s="22" t="n">
@@ -6405,7 +6414,7 @@
       <c r="H89" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I89" s="13" t="s">
+      <c r="I89" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J89" s="23" t="n">
@@ -6419,7 +6428,7 @@
         <v>18991</v>
       </c>
       <c r="M89" s="17"/>
-      <c r="N89" s="46" t="n">
+      <c r="N89" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O89" s="28" t="n">
@@ -6434,11 +6443,11 @@
       </c>
       <c r="R89" s="22"/>
     </row>
-    <row r="90" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="10" t="s">
+    <row r="90" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C90" s="22" t="n">
@@ -6459,7 +6468,7 @@
       <c r="H90" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I90" s="13" t="s">
+      <c r="I90" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J90" s="23" t="n">
@@ -6473,7 +6482,7 @@
         <v>20776</v>
       </c>
       <c r="M90" s="17"/>
-      <c r="N90" s="46" t="n">
+      <c r="N90" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O90" s="28" t="n">
@@ -6488,11 +6497,11 @@
       </c>
       <c r="R90" s="22"/>
     </row>
-    <row r="91" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C91" s="22" t="n">
@@ -6513,7 +6522,7 @@
       <c r="H91" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I91" s="13" t="s">
+      <c r="I91" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J91" s="23" t="n">
@@ -6527,7 +6536,7 @@
         <v>14280</v>
       </c>
       <c r="M91" s="17"/>
-      <c r="N91" s="46" t="n">
+      <c r="N91" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O91" s="28" t="n">
@@ -6542,11 +6551,11 @@
       </c>
       <c r="R91" s="22"/>
     </row>
-    <row r="92" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C92" s="22" t="n">
@@ -6567,7 +6576,7 @@
       <c r="H92" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I92" s="13" t="s">
+      <c r="I92" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J92" s="23" t="n">
@@ -6581,7 +6590,7 @@
         <v>16611</v>
       </c>
       <c r="M92" s="17"/>
-      <c r="N92" s="46" t="n">
+      <c r="N92" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O92" s="28" t="n">
@@ -6596,11 +6605,11 @@
       </c>
       <c r="R92" s="22"/>
     </row>
-    <row r="93" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C93" s="22" t="n">
@@ -6621,7 +6630,7 @@
       <c r="H93" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I93" s="13" t="s">
+      <c r="I93" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J93" s="23" t="n">
@@ -6635,7 +6644,7 @@
         <v>18193</v>
       </c>
       <c r="M93" s="17"/>
-      <c r="N93" s="46" t="n">
+      <c r="N93" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O93" s="28" t="n">
@@ -6650,11 +6659,11 @@
       </c>
       <c r="R93" s="22"/>
     </row>
-    <row r="94" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C94" s="22" t="n">
@@ -6675,7 +6684,7 @@
       <c r="H94" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="I94" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J94" s="23" t="n">
@@ -6689,7 +6698,7 @@
         <v>7000</v>
       </c>
       <c r="M94" s="17"/>
-      <c r="N94" s="46" t="n">
+      <c r="N94" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O94" s="28" t="n">
@@ -6704,11 +6713,11 @@
       </c>
       <c r="R94" s="22"/>
     </row>
-    <row r="95" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C95" s="22" t="n">
@@ -6729,7 +6738,7 @@
       <c r="H95" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I95" s="13" t="s">
+      <c r="I95" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J95" s="23" t="n">
@@ -6743,7 +6752,7 @@
         <v>8000</v>
       </c>
       <c r="M95" s="17"/>
-      <c r="N95" s="46" t="n">
+      <c r="N95" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O95" s="28" t="n">
@@ -6756,13 +6765,13 @@
       <c r="Q95" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R95" s="55"/>
-    </row>
-    <row r="96" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R95" s="57"/>
+    </row>
+    <row r="96" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="B96" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C96" s="22" t="n">
@@ -6783,7 +6792,7 @@
       <c r="H96" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I96" s="13" t="s">
+      <c r="I96" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J96" s="23" t="n">
@@ -6797,7 +6806,7 @@
         <v>8000</v>
       </c>
       <c r="M96" s="17"/>
-      <c r="N96" s="46" t="n">
+      <c r="N96" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O96" s="28" t="n">
@@ -6810,11 +6819,11 @@
       <c r="Q96" s="22"/>
       <c r="R96" s="22"/>
     </row>
-    <row r="97" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="B97" s="11" t="s">
+      <c r="B97" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C97" s="22" t="n">
@@ -6835,7 +6844,7 @@
       <c r="H97" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I97" s="13" t="s">
+      <c r="I97" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J97" s="23" t="n">
@@ -6849,7 +6858,7 @@
         <v>11934</v>
       </c>
       <c r="M97" s="17"/>
-      <c r="N97" s="46" t="n">
+      <c r="N97" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O97" s="28" t="n">
@@ -6864,11 +6873,11 @@
       </c>
       <c r="R97" s="22"/>
     </row>
-    <row r="98" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B98" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C98" s="22" t="n">
@@ -6889,7 +6898,7 @@
       <c r="H98" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I98" s="13" t="s">
+      <c r="I98" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J98" s="23" t="n">
@@ -6903,7 +6912,7 @@
         <v>11719.5</v>
       </c>
       <c r="M98" s="17"/>
-      <c r="N98" s="46" t="n">
+      <c r="N98" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O98" s="28" t="n">
@@ -6916,13 +6925,13 @@
       <c r="Q98" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R98" s="47"/>
-    </row>
-    <row r="99" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R98" s="49"/>
+    </row>
+    <row r="99" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C99" s="22" t="n">
@@ -6943,7 +6952,7 @@
       <c r="H99" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I99" s="13" t="s">
+      <c r="I99" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J99" s="23" t="n">
@@ -6957,7 +6966,7 @@
         <v>22080.5</v>
       </c>
       <c r="M99" s="17"/>
-      <c r="N99" s="46" t="n">
+      <c r="N99" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O99" s="28" t="n">
@@ -6970,13 +6979,13 @@
       <c r="Q99" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="R99" s="47"/>
-    </row>
-    <row r="100" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R99" s="49"/>
+    </row>
+    <row r="100" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C100" s="22" t="n">
@@ -6997,7 +7006,7 @@
       <c r="H100" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I100" s="13" t="s">
+      <c r="I100" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J100" s="23" t="n">
@@ -7011,7 +7020,7 @@
         <v>15496</v>
       </c>
       <c r="M100" s="17"/>
-      <c r="N100" s="46" t="n">
+      <c r="N100" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O100" s="28" t="n">
@@ -7024,13 +7033,13 @@
       <c r="Q100" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R100" s="47"/>
-    </row>
-    <row r="101" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R100" s="49"/>
+    </row>
+    <row r="101" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C101" s="22" t="n">
@@ -7051,7 +7060,7 @@
       <c r="H101" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I101" s="13" t="s">
+      <c r="I101" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J101" s="23" t="n">
@@ -7065,7 +7074,7 @@
         <v>28307.5</v>
       </c>
       <c r="M101" s="17"/>
-      <c r="N101" s="46" t="n">
+      <c r="N101" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O101" s="28" t="n">
@@ -7080,11 +7089,11 @@
       </c>
       <c r="R101" s="22"/>
     </row>
-    <row r="102" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C102" s="22" t="n">
@@ -7105,7 +7114,7 @@
       <c r="H102" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I102" s="13" t="s">
+      <c r="I102" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J102" s="23" t="n">
@@ -7119,7 +7128,7 @@
         <v>17771</v>
       </c>
       <c r="M102" s="17"/>
-      <c r="N102" s="46" t="n">
+      <c r="N102" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O102" s="28" t="n">
@@ -7132,13 +7141,13 @@
       <c r="Q102" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R102" s="47"/>
-    </row>
-    <row r="103" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R102" s="49"/>
+    </row>
+    <row r="103" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C103" s="22" t="n">
@@ -7159,7 +7168,7 @@
       <c r="H103" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I103" s="13" t="s">
+      <c r="I103" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J103" s="23" t="n">
@@ -7173,7 +7182,7 @@
         <v>14059.5</v>
       </c>
       <c r="M103" s="17"/>
-      <c r="N103" s="46" t="n">
+      <c r="N103" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O103" s="28" t="n">
@@ -7188,11 +7197,11 @@
       </c>
       <c r="R103" s="22"/>
     </row>
-    <row r="104" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C104" s="22" t="n">
@@ -7213,7 +7222,7 @@
       <c r="H104" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I104" s="13" t="s">
+      <c r="I104" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J104" s="23" t="n">
@@ -7227,7 +7236,7 @@
         <v>17914</v>
       </c>
       <c r="M104" s="17"/>
-      <c r="N104" s="46" t="n">
+      <c r="N104" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O104" s="28" t="n">
@@ -7242,11 +7251,11 @@
       </c>
       <c r="R104" s="22"/>
     </row>
-    <row r="105" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="B105" s="11" t="s">
+      <c r="B105" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C105" s="22" t="n">
@@ -7267,7 +7276,7 @@
       <c r="H105" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I105" s="13" t="s">
+      <c r="I105" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J105" s="23" t="n">
@@ -7281,7 +7290,7 @@
         <v>16932.5</v>
       </c>
       <c r="M105" s="17"/>
-      <c r="N105" s="46" t="n">
+      <c r="N105" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O105" s="28" t="n">
@@ -7296,11 +7305,11 @@
       </c>
       <c r="R105" s="22"/>
     </row>
-    <row r="106" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B106" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C106" s="22" t="n">
@@ -7321,7 +7330,7 @@
       <c r="H106" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I106" s="13" t="s">
+      <c r="I106" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J106" s="23" t="n">
@@ -7335,7 +7344,7 @@
         <v>16783</v>
       </c>
       <c r="M106" s="17"/>
-      <c r="N106" s="46" t="n">
+      <c r="N106" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O106" s="28" t="n">
@@ -7350,11 +7359,11 @@
       </c>
       <c r="R106" s="22"/>
     </row>
-    <row r="107" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="B107" s="11" t="s">
+      <c r="B107" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C107" s="22" t="n">
@@ -7375,7 +7384,7 @@
       <c r="H107" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I107" s="13" t="s">
+      <c r="I107" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J107" s="23" t="n">
@@ -7389,7 +7398,7 @@
         <v>18915</v>
       </c>
       <c r="M107" s="17"/>
-      <c r="N107" s="46" t="n">
+      <c r="N107" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O107" s="28" t="n">
@@ -7404,11 +7413,11 @@
       </c>
       <c r="R107" s="22"/>
     </row>
-    <row r="108" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="54" t="s">
+    <row r="108" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C108" s="22" t="n">
@@ -7429,7 +7438,7 @@
       <c r="H108" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I108" s="13" t="s">
+      <c r="I108" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J108" s="23" t="n">
@@ -7443,7 +7452,7 @@
         <v>40696.5</v>
       </c>
       <c r="M108" s="17"/>
-      <c r="N108" s="46" t="n">
+      <c r="N108" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O108" s="28" t="n">
@@ -7458,11 +7467,11 @@
       </c>
       <c r="R108" s="22"/>
     </row>
-    <row r="109" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="B109" s="11" t="s">
+      <c r="B109" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C109" s="22" t="n">
@@ -7483,7 +7492,7 @@
       <c r="H109" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I109" s="13" t="s">
+      <c r="I109" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J109" s="23" t="n">
@@ -7497,7 +7506,7 @@
         <v>15665</v>
       </c>
       <c r="M109" s="17"/>
-      <c r="N109" s="46" t="n">
+      <c r="N109" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O109" s="28" t="n">
@@ -7512,11 +7521,11 @@
       </c>
       <c r="R109" s="22"/>
     </row>
-    <row r="110" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C110" s="22" t="n">
@@ -7537,7 +7546,7 @@
       <c r="H110" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I110" s="13" t="s">
+      <c r="I110" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J110" s="23" t="n">
@@ -7551,7 +7560,7 @@
         <v>14059.5</v>
       </c>
       <c r="M110" s="17"/>
-      <c r="N110" s="46" t="n">
+      <c r="N110" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O110" s="28" t="n">
@@ -7564,11 +7573,11 @@
       <c r="Q110" s="20"/>
       <c r="R110" s="22"/>
     </row>
-    <row r="111" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C111" s="22" t="n">
@@ -7589,7 +7598,7 @@
       <c r="H111" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I111" s="13" t="s">
+      <c r="I111" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J111" s="23" t="n">
@@ -7603,7 +7612,7 @@
         <v>19292</v>
       </c>
       <c r="M111" s="17"/>
-      <c r="N111" s="46" t="n">
+      <c r="N111" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O111" s="28" t="n">
@@ -7618,11 +7627,11 @@
       </c>
       <c r="R111" s="22"/>
     </row>
-    <row r="112" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B112" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C112" s="22" t="n">
@@ -7643,7 +7652,7 @@
       <c r="H112" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I112" s="13" t="s">
+      <c r="I112" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J112" s="23" t="n">
@@ -7657,7 +7666,7 @@
         <v>13260</v>
       </c>
       <c r="M112" s="17"/>
-      <c r="N112" s="46" t="n">
+      <c r="N112" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O112" s="28" t="n">
@@ -7672,11 +7681,11 @@
       </c>
       <c r="R112" s="22"/>
     </row>
-    <row r="113" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="B113" s="11" t="s">
+      <c r="B113" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C113" s="22" t="n">
@@ -7697,7 +7706,7 @@
       <c r="H113" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I113" s="13" t="s">
+      <c r="I113" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J113" s="23" t="n">
@@ -7711,7 +7720,7 @@
         <v>15424.5</v>
       </c>
       <c r="M113" s="17"/>
-      <c r="N113" s="46" t="n">
+      <c r="N113" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O113" s="28" t="n">
@@ -7726,11 +7735,11 @@
       </c>
       <c r="R113" s="22"/>
     </row>
-    <row r="114" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="10" t="s">
+    <row r="114" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C114" s="12" t="n">
@@ -7751,7 +7760,7 @@
       <c r="H114" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I114" s="13" t="s">
+      <c r="I114" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J114" s="23" t="n">
@@ -7765,7 +7774,7 @@
         <v>16893.5</v>
       </c>
       <c r="M114" s="17"/>
-      <c r="N114" s="46" t="n">
+      <c r="N114" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O114" s="28" t="n">
@@ -7780,11 +7789,11 @@
       </c>
       <c r="R114" s="12"/>
     </row>
-    <row r="115" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="B115" s="11" t="s">
+      <c r="B115" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C115" s="22" t="n">
@@ -7805,7 +7814,7 @@
       <c r="H115" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I115" s="13" t="s">
+      <c r="I115" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J115" s="23" t="n">
@@ -7819,7 +7828,7 @@
         <v>6500</v>
       </c>
       <c r="M115" s="23"/>
-      <c r="N115" s="56" t="n">
+      <c r="N115" s="58" t="n">
         <v>3</v>
       </c>
       <c r="O115" s="36" t="n">
@@ -7834,11 +7843,11 @@
       </c>
       <c r="R115" s="22"/>
     </row>
-    <row r="116" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C116" s="22"/>
@@ -7857,7 +7866,7 @@
       <c r="H116" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I116" s="13" t="s">
+      <c r="I116" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J116" s="23" t="n">
@@ -7871,7 +7880,7 @@
         <v>7600</v>
       </c>
       <c r="M116" s="23"/>
-      <c r="N116" s="56" t="n">
+      <c r="N116" s="58" t="n">
         <v>3</v>
       </c>
       <c r="O116" s="36" t="n">
@@ -7886,11 +7895,11 @@
       </c>
       <c r="R116" s="22"/>
     </row>
-    <row r="117" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="B117" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C117" s="22" t="n">
@@ -7911,7 +7920,7 @@
       <c r="H117" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I117" s="13" t="s">
+      <c r="I117" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J117" s="23" t="n">
@@ -7925,7 +7934,7 @@
         <v>7600</v>
       </c>
       <c r="M117" s="23"/>
-      <c r="N117" s="56" t="n">
+      <c r="N117" s="58" t="n">
         <v>3</v>
       </c>
       <c r="O117" s="36" t="n">
@@ -7940,9 +7949,9 @@
       </c>
       <c r="R117" s="22"/>
     </row>
-    <row r="118" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="57"/>
-      <c r="B118" s="11" t="s">
+    <row r="118" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="59"/>
+      <c r="B118" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C118" s="22" t="n">
@@ -7963,7 +7972,7 @@
       <c r="H118" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I118" s="13" t="s">
+      <c r="I118" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J118" s="23" t="n">
@@ -7977,7 +7986,7 @@
         <v>6500</v>
       </c>
       <c r="M118" s="17"/>
-      <c r="N118" s="46" t="n">
+      <c r="N118" s="48" t="n">
         <v>3</v>
       </c>
       <c r="O118" s="28" t="n">
@@ -7992,9 +8001,9 @@
       </c>
       <c r="R118" s="22"/>
     </row>
-    <row r="119" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="57"/>
-      <c r="B119" s="11" t="s">
+    <row r="119" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="59"/>
+      <c r="B119" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C119" s="22" t="n">
@@ -8015,7 +8024,7 @@
       <c r="H119" s="15" t="n">
         <v>42380</v>
       </c>
-      <c r="I119" s="13" t="s">
+      <c r="I119" s="15" t="s">
         <v>18</v>
       </c>
       <c r="J119" s="23" t="n">
@@ -8029,7 +8038,7 @@
         <v>6500</v>
       </c>
       <c r="M119" s="17"/>
-      <c r="N119" s="58" t="n">
+      <c r="N119" s="60" t="n">
         <v>3</v>
       </c>
       <c r="O119" s="28" t="n">
@@ -8044,36 +8053,36 @@
       </c>
       <c r="R119" s="22"/>
     </row>
-    <row r="120" s="1" customFormat="true" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="59"/>
-      <c r="B120" s="11"/>
+    <row r="120" s="2" customFormat="true" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="61"/>
+      <c r="B120" s="12"/>
       <c r="C120" s="22"/>
-      <c r="D120" s="60" t="s">
+      <c r="D120" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="E120" s="60"/>
-      <c r="F120" s="60"/>
-      <c r="G120" s="60"/>
-      <c r="H120" s="60"/>
-      <c r="I120" s="60"/>
-      <c r="J120" s="60"/>
-      <c r="K120" s="60"/>
-      <c r="L120" s="60"/>
-      <c r="M120" s="60"/>
-      <c r="N120" s="60"/>
-      <c r="O120" s="60"/>
-      <c r="P120" s="61"/>
+      <c r="E120" s="62"/>
+      <c r="F120" s="62"/>
+      <c r="G120" s="62"/>
+      <c r="H120" s="62"/>
+      <c r="I120" s="62"/>
+      <c r="J120" s="62"/>
+      <c r="K120" s="62"/>
+      <c r="L120" s="62"/>
+      <c r="M120" s="62"/>
+      <c r="N120" s="62"/>
+      <c r="O120" s="62"/>
+      <c r="P120" s="63"/>
       <c r="Q120" s="22"/>
       <c r="R120" s="22"/>
     </row>
-    <row r="121" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="62" t="s">
+    <row r="121" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="64" t="s">
         <v>296</v>
       </c>
-      <c r="B121" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C121" s="47" t="n">
+      <c r="B121" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" s="49" t="n">
         <v>25000</v>
       </c>
       <c r="D121" s="24" t="s">
@@ -8083,7 +8092,7 @@
       <c r="F121" s="25" t="n">
         <v>570</v>
       </c>
-      <c r="G121" s="63" t="s">
+      <c r="G121" s="65" t="s">
         <v>298</v>
       </c>
       <c r="H121" s="24"/>
@@ -8099,7 +8108,7 @@
         <v>142500</v>
       </c>
       <c r="M121" s="17"/>
-      <c r="N121" s="58" t="n">
+      <c r="N121" s="60" t="n">
         <v>3</v>
       </c>
       <c r="O121" s="28" t="n">
@@ -8109,19 +8118,19 @@
       <c r="P121" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="Q121" s="64" t="n">
+      <c r="Q121" s="66" t="n">
         <v>42737</v>
       </c>
       <c r="R121" s="22"/>
     </row>
-    <row r="122" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="62" t="s">
+    <row r="122" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="64" t="s">
         <v>296</v>
       </c>
-      <c r="B122" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C122" s="65" t="n">
+      <c r="B122" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" s="67" t="n">
         <v>245300</v>
       </c>
       <c r="D122" s="24" t="s">
@@ -8131,7 +8140,7 @@
       <c r="F122" s="25" t="n">
         <v>1186</v>
       </c>
-      <c r="G122" s="63" t="s">
+      <c r="G122" s="65" t="s">
         <v>298</v>
       </c>
       <c r="H122" s="24"/>
@@ -8147,7 +8156,7 @@
         <v>415100</v>
       </c>
       <c r="M122" s="17"/>
-      <c r="N122" s="58" t="n">
+      <c r="N122" s="60" t="n">
         <v>3</v>
       </c>
       <c r="O122" s="28" t="n">
@@ -8161,24 +8170,24 @@
       <c r="R122" s="22"/>
     </row>
     <row r="123" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="66"/>
-      <c r="B123" s="67"/>
-      <c r="C123" s="68"/>
-      <c r="D123" s="69"/>
-      <c r="E123" s="69"/>
-      <c r="F123" s="69"/>
-      <c r="G123" s="69"/>
-      <c r="H123" s="69"/>
-      <c r="I123" s="69"/>
-      <c r="J123" s="69"/>
-      <c r="K123" s="69"/>
-      <c r="L123" s="69"/>
-      <c r="M123" s="69"/>
-      <c r="N123" s="69"/>
-      <c r="O123" s="69"/>
-      <c r="P123" s="70"/>
-      <c r="Q123" s="71"/>
-      <c r="R123" s="68"/>
+      <c r="A123" s="68"/>
+      <c r="B123" s="69"/>
+      <c r="C123" s="70"/>
+      <c r="D123" s="71"/>
+      <c r="E123" s="71"/>
+      <c r="F123" s="71"/>
+      <c r="G123" s="71"/>
+      <c r="H123" s="71"/>
+      <c r="I123" s="71"/>
+      <c r="J123" s="71"/>
+      <c r="K123" s="71"/>
+      <c r="L123" s="71"/>
+      <c r="M123" s="71"/>
+      <c r="N123" s="71"/>
+      <c r="O123" s="71"/>
+      <c r="P123" s="72"/>
+      <c r="Q123" s="73"/>
+      <c r="R123" s="70"/>
     </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>